<commit_message>
83 pag document + changed some interface menu text
</commit_message>
<xml_diff>
--- a/Office documents/sm10.xlsx
+++ b/Office documents/sm10.xlsx
@@ -383,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K269"/>
+  <dimension ref="A1:K274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
-      <selection activeCell="N262" sqref="N262"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="L277" sqref="L277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4087,7 +4087,7 @@
     </row>
     <row r="101" spans="1:11">
       <c r="A101" s="1">
-        <f t="shared" ref="A101:B116" si="5">A100+1</f>
+        <f t="shared" ref="A101:B104" si="5">A100+1</f>
         <v>100</v>
       </c>
       <c r="B101">
@@ -5715,11 +5715,11 @@
     </row>
     <row r="145" spans="1:11">
       <c r="A145" s="1">
-        <f t="shared" ref="A145:A164" si="17">A144+1</f>
+        <f t="shared" ref="A145:A163" si="17">A144+1</f>
         <v>144</v>
       </c>
       <c r="B145">
-        <f t="shared" ref="B145:B164" si="18">B144-2</f>
+        <f t="shared" ref="B145:B163" si="18">B144-2</f>
         <v>136</v>
       </c>
       <c r="C145" s="1">
@@ -7745,7 +7745,7 @@
     </row>
     <row r="200" spans="1:11">
       <c r="A200" s="1">
-        <f t="shared" ref="A200:A238" si="26">A199+1</f>
+        <f t="shared" ref="A200:A263" si="26">A199+1</f>
         <v>199</v>
       </c>
       <c r="B200">
@@ -9118,7 +9118,7 @@
         <v>236</v>
       </c>
       <c r="B237">
-        <f t="shared" ref="B237:B238" si="31">B236-1</f>
+        <f t="shared" ref="B237:B240" si="31">B236-1</f>
         <v>31</v>
       </c>
       <c r="C237" s="1">
@@ -9188,17 +9188,18 @@
     </row>
     <row r="239" spans="1:11">
       <c r="A239" s="1">
-        <f t="shared" ref="A239" si="32">A238+1</f>
+        <f t="shared" si="26"/>
         <v>238</v>
       </c>
       <c r="B239">
+        <f>B237-1</f>
         <v>30</v>
       </c>
       <c r="C239" s="1">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="D239" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E239" s="1">
         <v>0</v>
@@ -9213,7 +9214,7 @@
         <v>0</v>
       </c>
       <c r="I239" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J239" s="1">
         <v>0</v>
@@ -9224,12 +9225,11 @@
     </row>
     <row r="240" spans="1:11">
       <c r="A240" s="1">
-        <f t="shared" ref="A240" si="33">A239+1</f>
+        <f t="shared" si="26"/>
         <v>239</v>
       </c>
       <c r="B240">
-        <f>B239-1</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C240" s="1">
         <v>100</v>
@@ -9261,18 +9261,17 @@
     </row>
     <row r="241" spans="1:11">
       <c r="A241" s="1">
-        <f t="shared" ref="A241:A250" si="34">A240+1</f>
+        <f t="shared" si="26"/>
         <v>240</v>
       </c>
       <c r="B241">
-        <f t="shared" ref="B241:B250" si="35">B240-1</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C241" s="1">
         <v>100</v>
       </c>
       <c r="D241" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E241" s="1">
         <v>0</v>
@@ -9298,12 +9297,11 @@
     </row>
     <row r="242" spans="1:11">
       <c r="A242" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="26"/>
         <v>241</v>
       </c>
       <c r="B242">
-        <f t="shared" si="35"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C242" s="1">
         <v>100</v>
@@ -9335,12 +9333,11 @@
     </row>
     <row r="243" spans="1:11">
       <c r="A243" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="26"/>
         <v>242</v>
       </c>
       <c r="B243">
-        <f t="shared" si="35"/>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C243" s="1">
         <v>100</v>
@@ -9361,7 +9358,7 @@
         <v>0</v>
       </c>
       <c r="I243" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J243" s="1">
         <v>0</v>
@@ -9372,12 +9369,12 @@
     </row>
     <row r="244" spans="1:11">
       <c r="A244" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="26"/>
         <v>243</v>
       </c>
       <c r="B244">
-        <f t="shared" si="35"/>
-        <v>25</v>
+        <f>B243-1</f>
+        <v>29</v>
       </c>
       <c r="C244" s="1">
         <v>100</v>
@@ -9409,12 +9406,12 @@
     </row>
     <row r="245" spans="1:11">
       <c r="A245" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="26"/>
         <v>244</v>
       </c>
       <c r="B245">
-        <f t="shared" si="35"/>
-        <v>24</v>
+        <f t="shared" ref="B245:B254" si="32">B244-1</f>
+        <v>28</v>
       </c>
       <c r="C245" s="1">
         <v>100</v>
@@ -9446,12 +9443,12 @@
     </row>
     <row r="246" spans="1:11">
       <c r="A246" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="26"/>
         <v>245</v>
       </c>
       <c r="B246">
-        <f t="shared" si="35"/>
-        <v>23</v>
+        <f t="shared" si="32"/>
+        <v>27</v>
       </c>
       <c r="C246" s="1">
         <v>100</v>
@@ -9483,12 +9480,12 @@
     </row>
     <row r="247" spans="1:11">
       <c r="A247" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="26"/>
         <v>246</v>
       </c>
       <c r="B247">
-        <f t="shared" si="35"/>
-        <v>22</v>
+        <f t="shared" si="32"/>
+        <v>26</v>
       </c>
       <c r="C247" s="1">
         <v>100</v>
@@ -9520,12 +9517,12 @@
     </row>
     <row r="248" spans="1:11">
       <c r="A248" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="26"/>
         <v>247</v>
       </c>
       <c r="B248">
-        <f t="shared" si="35"/>
-        <v>21</v>
+        <f t="shared" si="32"/>
+        <v>25</v>
       </c>
       <c r="C248" s="1">
         <v>100</v>
@@ -9557,12 +9554,12 @@
     </row>
     <row r="249" spans="1:11">
       <c r="A249" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="26"/>
         <v>248</v>
       </c>
       <c r="B249">
-        <f t="shared" si="35"/>
-        <v>20</v>
+        <f t="shared" si="32"/>
+        <v>24</v>
       </c>
       <c r="C249" s="1">
         <v>100</v>
@@ -9594,12 +9591,12 @@
     </row>
     <row r="250" spans="1:11">
       <c r="A250" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="26"/>
         <v>249</v>
       </c>
       <c r="B250">
-        <f t="shared" si="35"/>
-        <v>19</v>
+        <f t="shared" si="32"/>
+        <v>23</v>
       </c>
       <c r="C250" s="1">
         <v>100</v>
@@ -9631,12 +9628,12 @@
     </row>
     <row r="251" spans="1:11">
       <c r="A251" s="1">
-        <f t="shared" ref="A251:A269" si="36">A250+1</f>
+        <f t="shared" si="26"/>
         <v>250</v>
       </c>
       <c r="B251">
-        <f t="shared" ref="B251:B260" si="37">B250-1</f>
-        <v>18</v>
+        <f t="shared" si="32"/>
+        <v>22</v>
       </c>
       <c r="C251" s="1">
         <v>100</v>
@@ -9668,12 +9665,12 @@
     </row>
     <row r="252" spans="1:11">
       <c r="A252" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>251</v>
       </c>
       <c r="B252">
-        <f t="shared" si="37"/>
-        <v>17</v>
+        <f t="shared" si="32"/>
+        <v>21</v>
       </c>
       <c r="C252" s="1">
         <v>100</v>
@@ -9705,12 +9702,12 @@
     </row>
     <row r="253" spans="1:11">
       <c r="A253" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>252</v>
       </c>
       <c r="B253">
-        <f t="shared" si="37"/>
-        <v>16</v>
+        <f t="shared" si="32"/>
+        <v>20</v>
       </c>
       <c r="C253" s="1">
         <v>100</v>
@@ -9742,12 +9739,12 @@
     </row>
     <row r="254" spans="1:11">
       <c r="A254" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>253</v>
       </c>
       <c r="B254">
-        <f t="shared" si="37"/>
-        <v>15</v>
+        <f t="shared" si="32"/>
+        <v>19</v>
       </c>
       <c r="C254" s="1">
         <v>100</v>
@@ -9779,12 +9776,12 @@
     </row>
     <row r="255" spans="1:11">
       <c r="A255" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>254</v>
       </c>
       <c r="B255">
-        <f t="shared" si="37"/>
-        <v>14</v>
+        <f t="shared" ref="B255:B264" si="33">B254-1</f>
+        <v>18</v>
       </c>
       <c r="C255" s="1">
         <v>100</v>
@@ -9816,12 +9813,12 @@
     </row>
     <row r="256" spans="1:11">
       <c r="A256" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>255</v>
       </c>
       <c r="B256">
-        <f t="shared" si="37"/>
-        <v>13</v>
+        <f t="shared" si="33"/>
+        <v>17</v>
       </c>
       <c r="C256" s="1">
         <v>100</v>
@@ -9853,12 +9850,12 @@
     </row>
     <row r="257" spans="1:11">
       <c r="A257" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>256</v>
       </c>
       <c r="B257">
-        <f t="shared" si="37"/>
-        <v>12</v>
+        <f t="shared" si="33"/>
+        <v>16</v>
       </c>
       <c r="C257" s="1">
         <v>100</v>
@@ -9890,12 +9887,12 @@
     </row>
     <row r="258" spans="1:11">
       <c r="A258" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>257</v>
       </c>
       <c r="B258">
-        <f t="shared" si="37"/>
-        <v>11</v>
+        <f t="shared" si="33"/>
+        <v>15</v>
       </c>
       <c r="C258" s="1">
         <v>100</v>
@@ -9927,12 +9924,12 @@
     </row>
     <row r="259" spans="1:11">
       <c r="A259" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>258</v>
       </c>
       <c r="B259">
-        <f t="shared" si="37"/>
-        <v>10</v>
+        <f t="shared" si="33"/>
+        <v>14</v>
       </c>
       <c r="C259" s="1">
         <v>100</v>
@@ -9964,12 +9961,12 @@
     </row>
     <row r="260" spans="1:11">
       <c r="A260" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>259</v>
       </c>
       <c r="B260">
-        <f t="shared" si="37"/>
-        <v>9</v>
+        <f t="shared" si="33"/>
+        <v>13</v>
       </c>
       <c r="C260" s="1">
         <v>100</v>
@@ -10001,12 +9998,12 @@
     </row>
     <row r="261" spans="1:11">
       <c r="A261" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>260</v>
       </c>
       <c r="B261">
-        <f>B260-1</f>
-        <v>8</v>
+        <f t="shared" si="33"/>
+        <v>12</v>
       </c>
       <c r="C261" s="1">
         <v>100</v>
@@ -10038,12 +10035,12 @@
     </row>
     <row r="262" spans="1:11">
       <c r="A262" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>261</v>
       </c>
       <c r="B262">
-        <f t="shared" ref="B262:B265" si="38">B261-1</f>
-        <v>7</v>
+        <f t="shared" si="33"/>
+        <v>11</v>
       </c>
       <c r="C262" s="1">
         <v>100</v>
@@ -10075,12 +10072,12 @@
     </row>
     <row r="263" spans="1:11">
       <c r="A263" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="26"/>
         <v>262</v>
       </c>
       <c r="B263">
-        <f t="shared" si="38"/>
-        <v>6</v>
+        <f t="shared" si="33"/>
+        <v>10</v>
       </c>
       <c r="C263" s="1">
         <v>100</v>
@@ -10112,12 +10109,12 @@
     </row>
     <row r="264" spans="1:11">
       <c r="A264" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" ref="A264:A274" si="34">A263+1</f>
         <v>263</v>
       </c>
       <c r="B264">
-        <f t="shared" si="38"/>
-        <v>5</v>
+        <f t="shared" si="33"/>
+        <v>9</v>
       </c>
       <c r="C264" s="1">
         <v>100</v>
@@ -10149,12 +10146,12 @@
     </row>
     <row r="265" spans="1:11">
       <c r="A265" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>264</v>
       </c>
       <c r="B265">
-        <f t="shared" si="38"/>
-        <v>4</v>
+        <f>B264-1</f>
+        <v>8</v>
       </c>
       <c r="C265" s="1">
         <v>100</v>
@@ -10186,12 +10183,12 @@
     </row>
     <row r="266" spans="1:11">
       <c r="A266" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>265</v>
       </c>
       <c r="B266">
-        <f>B265-1</f>
-        <v>3</v>
+        <f t="shared" ref="B266:B269" si="35">B265-1</f>
+        <v>7</v>
       </c>
       <c r="C266" s="1">
         <v>100</v>
@@ -10223,12 +10220,12 @@
     </row>
     <row r="267" spans="1:11">
       <c r="A267" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>266</v>
       </c>
       <c r="B267">
-        <f t="shared" ref="B267:B269" si="39">B266-1</f>
-        <v>2</v>
+        <f t="shared" si="35"/>
+        <v>6</v>
       </c>
       <c r="C267" s="1">
         <v>100</v>
@@ -10260,12 +10257,12 @@
     </row>
     <row r="268" spans="1:11">
       <c r="A268" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="34"/>
         <v>267</v>
       </c>
       <c r="B268">
-        <f t="shared" si="39"/>
-        <v>1</v>
+        <f t="shared" si="35"/>
+        <v>5</v>
       </c>
       <c r="C268" s="1">
         <v>100</v>
@@ -10297,38 +10294,222 @@
     </row>
     <row r="269" spans="1:11">
       <c r="A269" s="1">
+        <f t="shared" si="34"/>
+        <v>268</v>
+      </c>
+      <c r="B269">
+        <f t="shared" si="35"/>
+        <v>4</v>
+      </c>
+      <c r="C269" s="1">
+        <v>100</v>
+      </c>
+      <c r="D269" s="1">
+        <v>0</v>
+      </c>
+      <c r="E269" s="1">
+        <v>0</v>
+      </c>
+      <c r="F269" s="1">
+        <v>0</v>
+      </c>
+      <c r="G269" s="1">
+        <v>0</v>
+      </c>
+      <c r="H269" s="1">
+        <v>0</v>
+      </c>
+      <c r="I269" s="1">
+        <v>0</v>
+      </c>
+      <c r="J269" s="1">
+        <v>0</v>
+      </c>
+      <c r="K269" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:11">
+      <c r="A270" s="1">
+        <f t="shared" si="34"/>
+        <v>269</v>
+      </c>
+      <c r="B270">
+        <f>B269-1</f>
+        <v>3</v>
+      </c>
+      <c r="C270" s="1">
+        <v>100</v>
+      </c>
+      <c r="D270" s="1">
+        <v>0</v>
+      </c>
+      <c r="E270" s="1">
+        <v>0</v>
+      </c>
+      <c r="F270" s="1">
+        <v>0</v>
+      </c>
+      <c r="G270" s="1">
+        <v>0</v>
+      </c>
+      <c r="H270" s="1">
+        <v>0</v>
+      </c>
+      <c r="I270" s="1">
+        <v>0</v>
+      </c>
+      <c r="J270" s="1">
+        <v>0</v>
+      </c>
+      <c r="K270" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:11">
+      <c r="A271" s="1">
+        <f t="shared" si="34"/>
+        <v>270</v>
+      </c>
+      <c r="B271">
+        <f t="shared" ref="B271:B274" si="36">B270-1</f>
+        <v>2</v>
+      </c>
+      <c r="C271" s="1">
+        <v>100</v>
+      </c>
+      <c r="D271" s="1">
+        <v>0</v>
+      </c>
+      <c r="E271" s="1">
+        <v>0</v>
+      </c>
+      <c r="F271" s="1">
+        <v>0</v>
+      </c>
+      <c r="G271" s="1">
+        <v>0</v>
+      </c>
+      <c r="H271" s="1">
+        <v>0</v>
+      </c>
+      <c r="I271" s="1">
+        <v>0</v>
+      </c>
+      <c r="J271" s="1">
+        <v>0</v>
+      </c>
+      <c r="K271" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:11">
+      <c r="A272" s="1">
+        <f t="shared" si="34"/>
+        <v>271</v>
+      </c>
+      <c r="B272">
         <f t="shared" si="36"/>
-        <v>268</v>
-      </c>
-      <c r="B269">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="C269" s="1">
-        <v>100</v>
-      </c>
-      <c r="D269" s="1">
-        <v>0</v>
-      </c>
-      <c r="E269" s="1">
-        <v>0</v>
-      </c>
-      <c r="F269" s="1">
-        <v>0</v>
-      </c>
-      <c r="G269" s="1">
-        <v>0</v>
-      </c>
-      <c r="H269" s="1">
-        <v>0</v>
-      </c>
-      <c r="I269" s="1">
-        <v>0</v>
-      </c>
-      <c r="J269" s="1">
-        <v>0</v>
-      </c>
-      <c r="K269" s="1">
+        <v>1</v>
+      </c>
+      <c r="C272" s="1">
+        <v>100</v>
+      </c>
+      <c r="D272" s="1">
+        <v>0</v>
+      </c>
+      <c r="E272" s="1">
+        <v>0</v>
+      </c>
+      <c r="F272" s="1">
+        <v>0</v>
+      </c>
+      <c r="G272" s="1">
+        <v>0</v>
+      </c>
+      <c r="H272" s="1">
+        <v>0</v>
+      </c>
+      <c r="I272" s="1">
+        <v>0</v>
+      </c>
+      <c r="J272" s="1">
+        <v>0</v>
+      </c>
+      <c r="K272" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11">
+      <c r="A273" s="1">
+        <f t="shared" si="34"/>
+        <v>272</v>
+      </c>
+      <c r="B273">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="C273" s="1">
+        <v>100</v>
+      </c>
+      <c r="D273" s="1">
+        <v>0</v>
+      </c>
+      <c r="E273" s="1">
+        <v>0</v>
+      </c>
+      <c r="F273" s="1">
+        <v>0</v>
+      </c>
+      <c r="G273" s="1">
+        <v>0</v>
+      </c>
+      <c r="H273" s="1">
+        <v>0</v>
+      </c>
+      <c r="I273" s="1">
+        <v>0</v>
+      </c>
+      <c r="J273" s="1">
+        <v>0</v>
+      </c>
+      <c r="K273" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11">
+      <c r="A274" s="1">
+        <f t="shared" si="34"/>
+        <v>273</v>
+      </c>
+      <c r="B274">
+        <v>0</v>
+      </c>
+      <c r="C274" s="1">
+        <v>100</v>
+      </c>
+      <c r="D274" s="1">
+        <v>0</v>
+      </c>
+      <c r="E274" s="1">
+        <v>0</v>
+      </c>
+      <c r="F274" s="1">
+        <v>0</v>
+      </c>
+      <c r="G274" s="1">
+        <v>0</v>
+      </c>
+      <c r="H274" s="1">
+        <v>0</v>
+      </c>
+      <c r="I274" s="1">
+        <v>0</v>
+      </c>
+      <c r="J274" s="1">
+        <v>0</v>
+      </c>
+      <c r="K274" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>